<commit_message>
Add more verify for Log Out step
- Name & Text
</commit_message>
<xml_diff>
--- a/Android/Results/MobileTestResults.xlsx
+++ b/Android/Results/MobileTestResults.xlsx
@@ -367,9 +367,9 @@
           <t>Login by a registered email</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>

</xml_diff>